<commit_message>
Increase teemo scoring for teemo question
</commit_message>
<xml_diff>
--- a/championData.xlsx
+++ b/championData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\ChampionPickerApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6890D303-01FD-4D52-9EF3-CCD2BF5CE217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774F90BA-8815-4D4C-806F-78D90D0D4170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1422,9 +1422,7 @@
         <left style="thin">
           <color rgb="FFBFBFBF"/>
         </left>
-        <right style="thin">
-          <color rgb="FFBFBFBF"/>
-        </right>
+        <right/>
         <top style="thin">
           <color rgb="FFBFBFBF"/>
         </top>
@@ -1456,7 +1454,9 @@
         <left style="thin">
           <color rgb="FFBFBFBF"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color rgb="FFBFBFBF"/>
+        </right>
         <top style="thin">
           <color rgb="FFBFBFBF"/>
         </top>
@@ -1544,9 +1544,9 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataDxfId="1"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10" dataDxfId="0"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12"/>
   </tableColumns>
@@ -1755,10 +1755,10 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="L113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomRight" activeCell="M133" sqref="M133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7247,7 +7247,7 @@
         <v>1</v>
       </c>
       <c r="M133" s="13">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="134" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>